<commit_message>
Excel with test data modified
</commit_message>
<xml_diff>
--- a/data/Schnittstellenpartner.xlsx
+++ b/data/Schnittstellenpartner.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcu\Documents\Bewerbung\Bewerbung_2025\ApplyFor\20250709_BLB_Python\Präsentation_2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcu\Documents\Bewerbung\Bewerbung_2025\Workplace\converter_xlsx_json\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEEA5198-35C0-424C-8577-87FCDBAA7AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE20F3BE-A308-4D3E-A795-485BC3F119CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -100,17 +100,28 @@
     <definedName name="_xlnm.Print_Area" localSheetId="10">SST_8!$A:$B</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="11">SST_9!$A:$B</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2209" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2227" uniqueCount="401">
   <si>
     <t>Datenfeldname</t>
   </si>
@@ -1207,9 +1218,6 @@
     <t>Feldname Excel</t>
   </si>
   <si>
-    <t>Attributname JSON</t>
-  </si>
-  <si>
     <t>SST_NAME</t>
   </si>
   <si>
@@ -1231,9 +1239,6 @@
     <t>SST_AUTH_METHOD</t>
   </si>
   <si>
-    <t>SST_AUTORISATION</t>
-  </si>
-  <si>
     <t>SST_CRYPTO</t>
   </si>
   <si>
@@ -1259,6 +1264,66 @@
   </si>
   <si>
     <t>PARTNER_2_RESPONSIBLE</t>
+  </si>
+  <si>
+    <t>sst_name</t>
+  </si>
+  <si>
+    <t>sst_version</t>
+  </si>
+  <si>
+    <t>sst_valid_from</t>
+  </si>
+  <si>
+    <t>sst_valid_to</t>
+  </si>
+  <si>
+    <t>sst_is_active</t>
+  </si>
+  <si>
+    <t>sst_responsible</t>
+  </si>
+  <si>
+    <t>sst_auth_method</t>
+  </si>
+  <si>
+    <t>sst_authorization</t>
+  </si>
+  <si>
+    <t>sst_crypto</t>
+  </si>
+  <si>
+    <t>sst_format</t>
+  </si>
+  <si>
+    <t>sst_trigger</t>
+  </si>
+  <si>
+    <t>sst_protocol</t>
+  </si>
+  <si>
+    <t>sst_transport</t>
+  </si>
+  <si>
+    <t>partner_1_system</t>
+  </si>
+  <si>
+    <t>partner_1_responsible</t>
+  </si>
+  <si>
+    <t>partner_2_system</t>
+  </si>
+  <si>
+    <t>partner_2_responsible</t>
+  </si>
+  <si>
+    <t>Attributname JSON (klein)</t>
+  </si>
+  <si>
+    <t>Attributname JSON (groß)</t>
+  </si>
+  <si>
+    <t>SST_AUTHORIZATION</t>
   </si>
 </sst>
 </file>
@@ -1647,7 +1712,7 @@
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:A18"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3479,163 +3544,219 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAD2534D-BF8E-44EF-BFB3-24F535E59B8C}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>364</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>398</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>381</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>382</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>383</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>384</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>385</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>386</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>387</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>388</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>389</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>19</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>390</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>21</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>391</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>392</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>25</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>393</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>27</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>394</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>28</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>395</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>396</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>382</v>
+        <v>397</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>380</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5315,7 +5436,7 @@
   <dimension ref="A1:Q41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A41" sqref="A41:Q41"/>
     </sheetView>
   </sheetViews>

</xml_diff>